<commit_message>
Applied sklearn logistic regression to solve visual data accuracy issue
</commit_message>
<xml_diff>
--- a/src/baseline_model/baseline_lr_model_results.xlsx
+++ b/src/baseline_model/baseline_lr_model_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCL_CS\Y3\COMP0029 Individual Project\Individual Project (90%)\UCL-FYP\src\baseline_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EA57D0-1BE5-4FD3-93A3-11A93C314AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EBB232-3AA7-439A-AA3E-1F377617445A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17355" yWindow="2370" windowWidth="16920" windowHeight="10755" xr2:uid="{449CD272-F864-49D6-AEEE-8295C86900CF}"/>
+    <workbookView xWindow="-20160" yWindow="4005" windowWidth="16920" windowHeight="10755" xr2:uid="{449CD272-F864-49D6-AEEE-8295C86900CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Mug</t>
   </si>
@@ -177,6 +177,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -184,9 +187,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -506,7 +506,7 @@
   <dimension ref="C2:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,21 +526,21 @@
     </row>
     <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="4" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="4" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -578,31 +578,31 @@
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="4">
         <v>92.5</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="4">
         <v>50.75</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <v>92.5</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4">
         <v>86.5</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="4">
         <v>84</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="4">
         <v>77.75</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="4">
         <v>84.5</v>
       </c>
     </row>
@@ -610,63 +610,63 @@
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="7">
-        <v>94.2</v>
-      </c>
-      <c r="E8" s="7">
-        <v>50.5</v>
-      </c>
-      <c r="F8" s="7">
-        <v>94.1</v>
-      </c>
-      <c r="G8" s="7">
-        <v>92.1</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="7">
-        <v>91.8</v>
-      </c>
-      <c r="J8" s="7">
-        <v>95.6</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" s="7">
-        <v>93.3</v>
+      <c r="D8" s="4">
+        <v>99</v>
+      </c>
+      <c r="E8" s="4">
+        <v>90.5</v>
+      </c>
+      <c r="F8" s="4">
+        <v>99</v>
+      </c>
+      <c r="G8" s="4">
+        <v>90.5</v>
+      </c>
+      <c r="H8" s="4">
+        <v>92.5</v>
+      </c>
+      <c r="I8" s="4">
+        <v>92</v>
+      </c>
+      <c r="J8" s="4">
+        <v>99.5</v>
+      </c>
+      <c r="K8" s="4">
+        <v>98</v>
+      </c>
+      <c r="L8" s="4">
+        <v>98.5</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="4">
         <v>80.5</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="4">
         <v>50</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="4">
         <v>77.75</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="4">
         <v>85.5</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="4">
         <v>85</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="4">
         <v>85</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="4">
         <v>86.75</v>
       </c>
     </row>

</xml_diff>